<commit_message>
add case about set global variable to check the connection
</commit_message>
<xml_diff>
--- a/src/test/resources/io.dingodb.test/testdata/mysqlcases/protocol/mysql_protocol_cases.xlsx
+++ b/src/test/resources/io.dingodb.test/testdata/mysqlcases/protocol/mysql_protocol_cases.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="143">
   <si>
     <t>TestID</t>
   </si>
@@ -451,10 +451,6 @@
     <t>protocol_026</t>
   </si>
   <si>
-    <t>set wait_timeout=120</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>show variables like 'wait%'</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -512,6 +508,24 @@
     <t>create table mtest_5_sh_fi(id int, name varchar(20) not null default 'zhangsan', age int default 18, amount double not null default 99.99, price float, address varchar(255) null default 'BJ No.18',
 birthday date not null default '1970-01-01', create_time time default null, update_time timestamp default '2023-05-25 00:00:00', is_delete boolean not null, user_info any, primary key (id))</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>protocol_028</t>
+  </si>
+  <si>
+    <t>设置全局变量后验证登录</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>set wait_timeout=120</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>set global wait_timeout=60</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>connection</t>
   </si>
 </sst>
 </file>
@@ -881,10 +895,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K28"/>
+  <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -984,10 +998,10 @@
         <v>16</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>25</v>
@@ -1016,10 +1030,10 @@
         <v>20</v>
       </c>
       <c r="H4" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>128</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>129</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>26</v>
@@ -1248,10 +1262,10 @@
         <v>47</v>
       </c>
       <c r="H12" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="I12" s="2" t="s">
         <v>136</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>137</v>
       </c>
       <c r="J12" s="2" t="s">
         <v>68</v>
@@ -1393,7 +1407,7 @@
         <v>92</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I17" s="2" t="s">
         <v>93</v>
@@ -1445,13 +1459,13 @@
         <v>15</v>
       </c>
       <c r="H19" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="I19" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="I19" s="2" t="s">
+      <c r="J19" s="2" t="s">
         <v>124</v>
-      </c>
-      <c r="J19" s="2" t="s">
-        <v>125</v>
       </c>
       <c r="K19" s="6" t="s">
         <v>8</v>
@@ -1626,32 +1640,52 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A28" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" s="6" t="s">
         <v>130</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>131</v>
       </c>
       <c r="D28" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E28" s="6"/>
       <c r="F28" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="H28" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="H28" s="6" t="s">
+      <c r="I28" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="I28" s="2" t="s">
+      <c r="J28" s="2" t="s">
         <v>134</v>
-      </c>
-      <c r="J28" s="2" t="s">
-        <v>135</v>
       </c>
       <c r="K28" s="1" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A29" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H29" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -1661,7 +1695,7 @@
       <formula1>"y,n"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K1048576">
-      <formula1>"csv_equals,csv_containsAll,string_equals,effected_rows_assert,table_assert,assertNull,justExec,SQLException"</formula1>
+      <formula1>"csv_equals,csv_containsAll,string_equals,effected_rows_assert,table_assert,assertNull,justExec,connection,SQLException"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update mysql protocol case data
</commit_message>
<xml_diff>
--- a/src/test/resources/io.dingodb.test/testdata/mysqlcases/protocol/mysql_protocol_cases.xlsx
+++ b/src/test/resources/io.dingodb.test/testdata/mysqlcases/protocol/mysql_protocol_cases.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="156">
   <si>
     <t>TestID</t>
   </si>
@@ -126,10 +126,6 @@
   </si>
   <si>
     <t>查看单分区表分区信息</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>create table protocol_004(id int, name varchar(32), age int, amount double, primary key(id))</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -343,10 +339,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>desc protocol_016</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Op_sql</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -498,6 +490,35 @@
   </si>
   <si>
     <t>show table protocol_011 distribution</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>protocol_028</t>
+  </si>
+  <si>
+    <t>设置全局变量后验证登录</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>set wait_timeout=120</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>set global wait_timeout=60</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>connection</t>
+  </si>
+  <si>
+    <t>protocol_029</t>
+  </si>
+  <si>
+    <t>查看hash分区表的分区信息</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>create table protocol_004(id int, name varchar(32), age int, amount double, primary key(id))</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -506,25 +527,94 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>protocol_028</t>
-  </si>
-  <si>
-    <t>设置全局变量后验证登录</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>set wait_timeout=120</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>set global wait_timeout=60</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>connection</t>
+    <t>src/test/resources/io.dingodb.test/testdata/mysqlcases/protocol/expectedresult/protocol_029.csv</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>查看表的描述信息</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>protocol_029</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>create table protocol_029
+(
+    id int,
+    name varchar(32),
+    age int,
+    gmt bigint,
+    price float,
+    amount double,
+    address varchar(255),
+    birthday date,
+    create_time time,
+    update_time timestamp,
+    zip_code varchar(20),
+    is_delete boolean,
+    feature float array not null,
+    user_info any,
+    feature_id bigint not null,
+    primary key (id, birthday),
+    index name_index (name) partition by hash partitions=10,
+    index feature_index vector(feature_id, feature) partition by hash partitions=5 parameters(type=hnsw, metricType=L2, dimension=64, efConstruction=40, nlinks=32)
+) partition by hash partitions=10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>show table protocol_029 distribution</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>create table protocol_016(id int auto_increment, acct_no varchar, tx_date date not null default '2020-10-01', tx_time time default '18:30:00', tx_type int default 1, tx_status boolean, tx_amt double,uble, tx_location varchar(255) default 'BJ', id_card_no varchar(18), phone varchar(11) not null, write_time timestamp default '2023-06-12 13:30:30', primary key(id, acct_no, tx_date))</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>protocol_030</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/mysqlcases/protocol/expectedresult/protocol_030.csv</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>protocol_030</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>desc protocol_030</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>desc protocol_016</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>create table protocol_030
+(
+    id int not null auto_increment,
+    name varchar(32),
+    age int,
+    gmt bigint,
+    price float,
+    amount double,
+    address varchar(255),
+    birthday date,
+    create_time time,
+    update_time timestamp,
+    zip_code varchar(20),
+    is_delete boolean,
+    feature float array not null,
+    user_info any,
+    feature_id bigint not null,
+    primary key (id, birthday),
+    index age_index (age) partition by range values (20),(55),(80),
+    index feature_index vector(feature_id, feature) partition by range values (20) parameters(type=hnsw, metricType=L2, dimension=64, efConstruction=40, nlinks=32)
+) partition by range values (200,'1990-01-01'),(400,'2000-01-01'),(600,'2010-01-01'),(800,'2020-01-01')</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HASH_Distribution</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -585,7 +675,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
@@ -594,6 +684,9 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -895,10 +988,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K29"/>
+  <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -910,7 +1003,7 @@
     <col min="5" max="5" width="15" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" style="6" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.75" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.375" style="6" customWidth="1"/>
+    <col min="8" max="8" width="48.125" style="6" customWidth="1"/>
     <col min="9" max="9" width="21.625" style="2" customWidth="1"/>
     <col min="10" max="10" width="20.625" style="2" customWidth="1"/>
     <col min="11" max="11" width="19.5" style="1" bestFit="1" customWidth="1"/>
@@ -940,7 +1033,7 @@
         <v>19</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="I1" s="7" t="s">
         <v>6</v>
@@ -981,7 +1074,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:11" ht="135" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
         <v>10</v>
       </c>
@@ -997,11 +1090,11 @@
       <c r="E3" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>136</v>
+      <c r="H3" s="8" t="s">
+        <v>142</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>25</v>
@@ -1030,10 +1123,10 @@
         <v>20</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>26</v>
@@ -1053,19 +1146,19 @@
         <v>30</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E5" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="I5" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="H5" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="I5" s="2" t="s">
+      <c r="J5" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>34</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>8</v>
@@ -1073,28 +1166,28 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A6" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H6" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="6" t="s">
+      <c r="I6" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D6" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="H6" s="6" t="s">
+      <c r="J6" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>38</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>8</v>
@@ -1102,28 +1195,28 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A7" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>42</v>
-      </c>
       <c r="D7" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I7" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="J7" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>57</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>8</v>
@@ -1131,28 +1224,28 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A8" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K8" s="6" t="s">
         <v>8</v>
@@ -1160,28 +1253,28 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A9" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K9" s="6" t="s">
         <v>8</v>
@@ -1189,28 +1282,28 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A10" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K10" s="6" t="s">
         <v>8</v>
@@ -1218,28 +1311,28 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A11" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K11" s="6" t="s">
         <v>8</v>
@@ -1247,28 +1340,28 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A12" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K12" s="6" t="s">
         <v>8</v>
@@ -1276,28 +1369,28 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A13" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K13" s="6" t="s">
         <v>8</v>
@@ -1305,28 +1398,28 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A14" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K14" s="6" t="s">
         <v>8</v>
@@ -1334,28 +1427,28 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A15" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="B15" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>80</v>
-      </c>
       <c r="D15" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K15" s="6" t="s">
         <v>8</v>
@@ -1363,28 +1456,28 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A16" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="B16" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>82</v>
-      </c>
       <c r="D16" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K16" s="6" t="s">
         <v>8</v>
@@ -1392,28 +1485,28 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A17" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>90</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>93</v>
+        <v>153</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="K17" s="1" t="s">
         <v>21</v>
@@ -1421,25 +1514,25 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A18" s="6" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>15</v>
       </c>
       <c r="H18" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="J18" s="2" t="s">
         <v>97</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>99</v>
       </c>
       <c r="K18" s="1" t="s">
         <v>8</v>
@@ -1447,25 +1540,25 @@
     </row>
     <row r="19" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A19" s="6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>15</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="K19" s="6" t="s">
         <v>8</v>
@@ -1473,196 +1566,196 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A20" s="6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E20" s="6"/>
       <c r="H20" s="6" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A21" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E21" s="6"/>
       <c r="H21" s="6" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K21" s="6" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A22" s="6" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D22" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E22" s="6"/>
       <c r="H22" s="6" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="K22" s="6" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A23" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D23" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E23" s="6"/>
       <c r="H23" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="K23" s="6" t="s">
         <v>116</v>
-      </c>
-      <c r="K23" s="6" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A24" s="6" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D24" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E24" s="6"/>
       <c r="H24" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="K24" s="6" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A25" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D25" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E25" s="6"/>
       <c r="H25" s="6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K25" s="6" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A26" s="6" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B26" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D26" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E26" s="6"/>
       <c r="H26" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="K26" s="6" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A27" s="6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B27" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D27" s="6" t="s">
         <v>15</v>
       </c>
       <c r="H27" s="6" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A28" s="6" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D28" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E28" s="6"/>
       <c r="F28" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="H28" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="I28" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="H28" s="6" t="s">
+      <c r="J28" s="2" t="s">
         <v>131</v>
-      </c>
-      <c r="I28" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="J28" s="2" t="s">
-        <v>133</v>
       </c>
       <c r="K28" s="1" t="s">
         <v>8</v>
@@ -1670,22 +1763,80 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A29" s="6" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B29" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D29" s="6" t="s">
         <v>15</v>
       </c>
       <c r="H29" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="337.5" x14ac:dyDescent="0.15">
+      <c r="A30" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="K29" s="1" t="s">
-        <v>141</v>
+      <c r="D30" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="H30" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="364.5" x14ac:dyDescent="0.15">
+      <c r="A31" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="H31" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="K31" s="6" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
remove the sleep time of index explain assertion
</commit_message>
<xml_diff>
--- a/src/test/resources/io.dingodb.test/testdata/mysqlcases/protocol/mysql_protocol_cases.xlsx
+++ b/src/test/resources/io.dingodb.test/testdata/mysqlcases/protocol/mysql_protocol_cases.xlsx
@@ -350,10 +350,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>set interactive_timeout=60</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>show variables like 'interactive_timeout'</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -497,10 +493,6 @@
   </si>
   <si>
     <t>设置全局变量后验证登录</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>set wait_timeout=120</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -615,6 +607,14 @@
   </si>
   <si>
     <t>HASH_Distribution</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>set interactive_timeout=14400</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>set wait_timeout=43200</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -990,8 +990,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1091,10 +1091,10 @@
         <v>16</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>25</v>
@@ -1123,10 +1123,10 @@
         <v>20</v>
       </c>
       <c r="H4" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>124</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>125</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>26</v>
@@ -1152,7 +1152,7 @@
         <v>31</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>32</v>
@@ -1355,10 +1355,10 @@
         <v>46</v>
       </c>
       <c r="H12" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="I12" s="2" t="s">
         <v>132</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>133</v>
       </c>
       <c r="J12" s="2" t="s">
         <v>67</v>
@@ -1500,10 +1500,10 @@
         <v>91</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="J17" s="2" t="s">
         <v>90</v>
@@ -1526,13 +1526,13 @@
         <v>15</v>
       </c>
       <c r="H18" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="I18" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="I18" s="2" t="s">
+      <c r="J18" s="2" t="s">
         <v>96</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>97</v>
       </c>
       <c r="K18" s="1" t="s">
         <v>8</v>
@@ -1540,7 +1540,7 @@
     </row>
     <row r="19" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A19" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>5</v>
@@ -1552,13 +1552,13 @@
         <v>15</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>136</v>
+        <v>155</v>
       </c>
       <c r="I19" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="J19" s="2" t="s">
         <v>121</v>
-      </c>
-      <c r="J19" s="2" t="s">
-        <v>122</v>
       </c>
       <c r="K19" s="6" t="s">
         <v>8</v>
@@ -1566,196 +1566,196 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A20" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E20" s="6"/>
       <c r="H20" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A21" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E21" s="6"/>
       <c r="H21" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K21" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A22" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D22" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E22" s="6"/>
       <c r="H22" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K22" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A23" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D23" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E23" s="6"/>
       <c r="H23" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K23" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A24" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D24" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E24" s="6"/>
       <c r="H24" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="K24" s="6" t="s">
         <v>115</v>
-      </c>
-      <c r="K24" s="6" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A25" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D25" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E25" s="6"/>
       <c r="H25" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K25" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A26" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B26" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D26" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E26" s="6"/>
       <c r="H26" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K26" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A27" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B27" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D27" s="6" t="s">
         <v>15</v>
       </c>
       <c r="H27" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A28" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" s="6" t="s">
         <v>126</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>127</v>
       </c>
       <c r="D28" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E28" s="6"/>
       <c r="F28" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="H28" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="H28" s="6" t="s">
+      <c r="I28" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="I28" s="2" t="s">
+      <c r="J28" s="2" t="s">
         <v>130</v>
-      </c>
-      <c r="J28" s="2" t="s">
-        <v>131</v>
       </c>
       <c r="K28" s="1" t="s">
         <v>8</v>
@@ -1763,48 +1763,48 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A29" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>134</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>135</v>
       </c>
       <c r="D29" s="6" t="s">
         <v>15</v>
       </c>
       <c r="H29" s="6" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="337.5" x14ac:dyDescent="0.15">
       <c r="A30" s="6" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B30" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E30" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="H30" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="I30" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="H30" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="I30" s="2" t="s">
-        <v>147</v>
-      </c>
       <c r="J30" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="K30" s="1" t="s">
         <v>8</v>
@@ -1812,28 +1812,28 @@
     </row>
     <row r="31" spans="1:11" ht="364.5" x14ac:dyDescent="0.15">
       <c r="A31" s="6" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B31" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D31" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="H31" s="8" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="K31" s="6" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
fix protocol case code
</commit_message>
<xml_diff>
--- a/src/test/resources/io.dingodb.test/testdata/mysqlcases/protocol/mysql_protocol_cases.xlsx
+++ b/src/test/resources/io.dingodb.test/testdata/mysqlcases/protocol/mysql_protocol_cases.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="166">
   <si>
     <t>TestID</t>
   </si>
@@ -344,14 +344,6 @@
   </si>
   <si>
     <t>protocol_017</t>
-  </si>
-  <si>
-    <t>设置变量值</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>show variables like 'interactive_timeout'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>src/test/resources/io.dingodb.test/testdata/mysqlcases/protocol/expectedresult/protocol_017.csv</t>
@@ -610,7 +602,47 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>set interactive_timeout=14400</t>
+    <t>protocol_031</t>
+  </si>
+  <si>
+    <t>查看编码变量</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>show variables like '%character%'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/mysqlcases/protocol/expectedresult/protocol_031.csv</t>
+  </si>
+  <si>
+    <t>protocol_032</t>
+  </si>
+  <si>
+    <t>设置编码变量</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>set names utf8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/mysqlcases/protocol/expectedresult/protocol_032.csv</t>
+  </si>
+  <si>
+    <t>设置变量值interactive_timeout</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>设置变量值wait_timeout</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>set global interactive_timeout=14400</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>show global variables like 'interactive_timeout'</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -618,32 +650,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>protocol_031</t>
-  </si>
-  <si>
-    <t>查看编码变量</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>show variables like '%character%'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>src/test/resources/io.dingodb.test/testdata/mysqlcases/protocol/expectedresult/protocol_031.csv</t>
-  </si>
-  <si>
-    <t>protocol_032</t>
-  </si>
-  <si>
-    <t>设置编码变量</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>set names utf8</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>src/test/resources/io.dingodb.test/testdata/mysqlcases/protocol/expectedresult/protocol_032.csv</t>
+    <t>n</t>
   </si>
 </sst>
 </file>
@@ -1018,8 +1025,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F40" sqref="F40"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1119,10 +1126,10 @@
         <v>16</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>25</v>
@@ -1151,10 +1158,10 @@
         <v>20</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>26</v>
@@ -1180,7 +1187,7 @@
         <v>31</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>32</v>
@@ -1383,10 +1390,10 @@
         <v>46</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="J12" s="2" t="s">
         <v>67</v>
@@ -1528,10 +1535,10 @@
         <v>91</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="J17" s="2" t="s">
         <v>90</v>
@@ -1548,19 +1555,19 @@
         <v>5</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>94</v>
+        <v>160</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>15</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>95</v>
+        <v>163</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="K18" s="1" t="s">
         <v>8</v>
@@ -1568,25 +1575,25 @@
     </row>
     <row r="19" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A19" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>5</v>
+        <v>165</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>94</v>
+        <v>161</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>15</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>155</v>
+        <v>164</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="K19" s="6" t="s">
         <v>8</v>
@@ -1594,196 +1601,196 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A20" s="6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E20" s="6"/>
       <c r="H20" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A21" s="6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E21" s="6"/>
       <c r="H21" s="6" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="K21" s="6" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A22" s="6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D22" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E22" s="6"/>
       <c r="H22" s="6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K22" s="6" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A23" s="6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D23" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E23" s="6"/>
       <c r="H23" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="K23" s="6" t="s">
         <v>113</v>
-      </c>
-      <c r="K23" s="6" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A24" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D24" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E24" s="6"/>
       <c r="H24" s="6" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K24" s="6" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A25" s="6" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D25" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E25" s="6"/>
       <c r="H25" s="6" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="K25" s="6" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A26" s="6" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B26" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D26" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E26" s="6"/>
       <c r="H26" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="K26" s="6" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A27" s="6" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B27" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D27" s="6" t="s">
         <v>15</v>
       </c>
       <c r="H27" s="6" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A28" s="6" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D28" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E28" s="6"/>
       <c r="F28" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="H28" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="I28" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="H28" s="6" t="s">
+      <c r="J28" s="2" t="s">
         <v>128</v>
-      </c>
-      <c r="I28" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="J28" s="2" t="s">
-        <v>130</v>
       </c>
       <c r="K28" s="1" t="s">
         <v>8</v>
@@ -1791,48 +1798,48 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A29" s="6" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B29" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D29" s="6" t="s">
         <v>15</v>
       </c>
       <c r="H29" s="6" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="337.5" x14ac:dyDescent="0.15">
       <c r="A30" s="6" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B30" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E30" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="H30" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="I30" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="H30" s="8" t="s">
-        <v>144</v>
-      </c>
-      <c r="I30" s="2" t="s">
-        <v>145</v>
-      </c>
       <c r="J30" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="K30" s="1" t="s">
         <v>8</v>
@@ -1840,28 +1847,28 @@
     </row>
     <row r="31" spans="1:11" ht="364.5" x14ac:dyDescent="0.15">
       <c r="A31" s="6" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B31" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D31" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="H31" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="K31" s="6" t="s">
         <v>21</v>
@@ -1869,22 +1876,22 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A32" s="6" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B32" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="D32" s="6" t="s">
         <v>15</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="K32" s="6" t="s">
         <v>21</v>
@@ -1892,25 +1899,25 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A33" s="6" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B33" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="D33" s="6" t="s">
         <v>15</v>
       </c>
       <c r="H33" s="6" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="K33" s="6" t="s">
         <v>21</v>

</xml_diff>